<commit_message>
add data source to paper figures
</commit_message>
<xml_diff>
--- a/outputs_report/Table_simSum_historical.xlsx
+++ b/outputs_report/Table_simSum_historical.xlsx
@@ -345,25 +345,25 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.12556966109173073</v>
+        <v>0.23970740326992024</v>
       </c>
       <c r="C5" t="n">
         <v>0.517</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.6535356635260239</v>
+        <v>-0.6060840550651159</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.27599607268647997</v>
+        <v>-0.196229634840153</v>
       </c>
       <c r="F5" t="n">
-        <v>0.09536002208510208</v>
+        <v>0.20691202397543695</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6104704337980977</v>
+        <v>0.7661123946570869</v>
       </c>
       <c r="H5" t="n">
-        <v>1.6099757864094923</v>
+        <v>1.851168629144542</v>
       </c>
     </row>
   </sheetData>
@@ -411,22 +411,22 @@
         <v>0.06555341590682408</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4933</v>
+        <v>0.4994</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04362494382315099</v>
+        <v>0.04363721101244466</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05699137157595631</v>
+        <v>0.0568792581878948</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06580877648283112</v>
+        <v>0.06556555449067433</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07492116363236292</v>
+        <v>0.07463659625828681</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08756290166043794</v>
+        <v>0.08802956058478767</v>
       </c>
     </row>
     <row r="3">
@@ -437,22 +437,22 @@
         <v>0.096320844630497</v>
       </c>
       <c r="C3" t="n">
-        <v>0.142</v>
+        <v>0.145</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09110125094786838</v>
+        <v>0.09093375997709403</v>
       </c>
       <c r="E3" t="n">
-        <v>0.09986901775711567</v>
+        <v>0.09972855014391979</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1064011381672044</v>
+        <v>0.10643499024242487</v>
       </c>
       <c r="G3" t="n">
-        <v>0.11354558088574518</v>
+        <v>0.11333968857606655</v>
       </c>
       <c r="H3" t="n">
-        <v>0.12356274041515744</v>
+        <v>0.1230834564037469</v>
       </c>
     </row>
     <row r="4">
@@ -463,22 +463,22 @@
         <v>0.595116859354557</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9093</v>
+        <v>0.9028</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.27012314996320186</v>
+        <v>-0.281157039799116</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.0011457116177368697</v>
+        <v>-0.006979241493880042</v>
       </c>
       <c r="F4" t="n">
-        <v>0.19010189242551834</v>
+        <v>0.18556782707050368</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3922178305802789</v>
+        <v>0.398419700386967</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6969959245860892</v>
+        <v>0.7031648335539682</v>
       </c>
     </row>
     <row r="5">
@@ -489,22 +489,22 @@
         <v>0.6319370379657605</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8822</v>
+        <v>0.8814</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.7746517888924525</v>
+        <v>-0.7642588622075719</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.4625490509458924</v>
+        <v>-0.45348283662630395</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.15602928488355383</v>
+        <v>-0.15711020900224804</v>
       </c>
       <c r="G5" t="n">
-        <v>0.21759826456773934</v>
+        <v>0.20493530999286758</v>
       </c>
       <c r="H5" t="n">
-        <v>1.0976953780626306</v>
+        <v>1.0636256397515187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>